<commit_message>
MZ 29092023 update privacyMetric Leakage
</commit_message>
<xml_diff>
--- a/examples/trainData/initialisation_report.xlsx
+++ b/examples/trainData/initialisation_report.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itssastar-my.sharepoint.com/personal/tanmz-bii_bii_a-star_edu_sg/Documents/DAR/synData/copula-tabular/examples/trainData/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_9A39C47A3FCA0303712D4C2B459D46B9639E7022" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD5F52AC-9D6C-4BF2-A264-9CC256B0AB2C}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="by Variable" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -457,10 +451,10 @@
     <t>Good,nan,Vgood,Fair,Excellent,Poor</t>
   </si>
   <si>
-    <t>Most,nan,Several,None</t>
-  </si>
-  <si>
-    <t>Several,nan,None,Most</t>
+    <t>Most,nan,Several</t>
+  </si>
+  <si>
+    <t>Several,nan,Most</t>
   </si>
   <si>
     <t>Yes,nan,No</t>
@@ -487,8 +481,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,21 +545,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -603,7 +589,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -637,7 +623,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -672,10 +657,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -848,18 +832,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="135.44140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -882,7 +862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -908,7 +888,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -934,7 +914,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -957,7 +937,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -980,7 +960,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1006,7 +986,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1023,13 +1003,13 @@
         <v>333</v>
       </c>
       <c r="F7">
-        <v>3.3300000000000003E-2</v>
+        <v>0.0333</v>
       </c>
       <c r="H7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1046,7 +1026,7 @@
         <v>5038</v>
       </c>
       <c r="F8">
-        <v>0.50380000000000003</v>
+        <v>0.5038</v>
       </c>
       <c r="G8" t="s">
         <v>93</v>
@@ -1055,7 +1035,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1078,7 +1058,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1101,7 +1081,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1118,13 +1098,13 @@
         <v>2779</v>
       </c>
       <c r="F11">
-        <v>0.27789999999999998</v>
+        <v>0.2779</v>
       </c>
       <c r="H11" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1141,13 +1121,13 @@
         <v>2769</v>
       </c>
       <c r="F12">
-        <v>0.27689999999999998</v>
+        <v>0.2769</v>
       </c>
       <c r="H12" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1164,13 +1144,13 @@
         <v>811</v>
       </c>
       <c r="F13">
-        <v>8.1100000000000005E-2</v>
+        <v>0.08110000000000001</v>
       </c>
       <c r="H13" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1187,7 +1167,7 @@
         <v>811</v>
       </c>
       <c r="F14">
-        <v>8.1100000000000005E-2</v>
+        <v>0.08110000000000001</v>
       </c>
       <c r="G14" t="s">
         <v>94</v>
@@ -1196,7 +1176,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1213,7 +1193,7 @@
         <v>726</v>
       </c>
       <c r="F15">
-        <v>7.2599999999999998E-2</v>
+        <v>0.0726</v>
       </c>
       <c r="G15" t="s">
         <v>95</v>
@@ -1222,7 +1202,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -1239,7 +1219,7 @@
         <v>69</v>
       </c>
       <c r="F16">
-        <v>6.8999999999999999E-3</v>
+        <v>0.0069</v>
       </c>
       <c r="G16" t="s">
         <v>96</v>
@@ -1248,7 +1228,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1265,13 +1245,13 @@
         <v>63</v>
       </c>
       <c r="F17">
-        <v>6.3E-3</v>
+        <v>0.0063</v>
       </c>
       <c r="H17" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -1288,13 +1268,13 @@
         <v>2229</v>
       </c>
       <c r="F18">
-        <v>0.22289999999999999</v>
+        <v>0.2229</v>
       </c>
       <c r="H18" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1311,7 +1291,7 @@
         <v>78</v>
       </c>
       <c r="F19">
-        <v>7.7999999999999996E-3</v>
+        <v>0.0078</v>
       </c>
       <c r="G19" t="s">
         <v>97</v>
@@ -1320,7 +1300,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -1337,7 +1317,7 @@
         <v>9457</v>
       </c>
       <c r="F20">
-        <v>0.94569999999999999</v>
+        <v>0.9457</v>
       </c>
       <c r="G20" t="s">
         <v>98</v>
@@ -1346,7 +1326,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -1363,7 +1343,7 @@
         <v>9912</v>
       </c>
       <c r="F21">
-        <v>0.99119999999999997</v>
+        <v>0.9912</v>
       </c>
       <c r="G21" t="s">
         <v>99</v>
@@ -1372,7 +1352,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -1389,7 +1369,7 @@
         <v>353</v>
       </c>
       <c r="F22">
-        <v>3.5299999999999998E-2</v>
+        <v>0.0353</v>
       </c>
       <c r="G22" t="s">
         <v>100</v>
@@ -1398,7 +1378,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -1415,7 +1395,7 @@
         <v>366</v>
       </c>
       <c r="F23">
-        <v>3.6600000000000001E-2</v>
+        <v>0.0366</v>
       </c>
       <c r="G23" t="s">
         <v>101</v>
@@ -1424,7 +1404,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -1441,13 +1421,13 @@
         <v>8726</v>
       </c>
       <c r="F24">
-        <v>0.87260000000000004</v>
+        <v>0.8726</v>
       </c>
       <c r="H24" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -1464,13 +1444,13 @@
         <v>397</v>
       </c>
       <c r="F25">
-        <v>3.9699999999999999E-2</v>
+        <v>0.0397</v>
       </c>
       <c r="H25" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
@@ -1487,7 +1467,7 @@
         <v>1437</v>
       </c>
       <c r="F26">
-        <v>0.14369999999999999</v>
+        <v>0.1437</v>
       </c>
       <c r="G26" t="s">
         <v>102</v>
@@ -1496,7 +1476,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -1522,7 +1502,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
@@ -1548,7 +1528,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
@@ -1565,7 +1545,7 @@
         <v>1763</v>
       </c>
       <c r="F29">
-        <v>0.17630000000000001</v>
+        <v>0.1763</v>
       </c>
       <c r="G29" t="s">
         <v>105</v>
@@ -1574,7 +1554,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
@@ -1591,7 +1571,7 @@
         <v>1763</v>
       </c>
       <c r="F30">
-        <v>0.17630000000000001</v>
+        <v>0.1763</v>
       </c>
       <c r="G30" t="s">
         <v>106</v>
@@ -1600,7 +1580,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
@@ -1617,7 +1597,7 @@
         <v>1647</v>
       </c>
       <c r="F31">
-        <v>0.16470000000000001</v>
+        <v>0.1647</v>
       </c>
       <c r="G31" t="s">
         <v>103</v>
@@ -1626,7 +1606,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
@@ -1643,7 +1623,7 @@
         <v>1647</v>
       </c>
       <c r="F32">
-        <v>0.16470000000000001</v>
+        <v>0.1647</v>
       </c>
       <c r="G32" t="s">
         <v>106</v>
@@ -1652,7 +1632,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
         <v>38</v>
       </c>
@@ -1669,7 +1649,7 @@
         <v>1635</v>
       </c>
       <c r="F33">
-        <v>0.16350000000000001</v>
+        <v>0.1635</v>
       </c>
       <c r="G33" t="s">
         <v>103</v>
@@ -1678,7 +1658,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
@@ -1695,7 +1675,7 @@
         <v>1635</v>
       </c>
       <c r="F34">
-        <v>0.16350000000000001</v>
+        <v>0.1635</v>
       </c>
       <c r="G34" t="s">
         <v>104</v>
@@ -1704,7 +1684,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
         <v>40</v>
       </c>
@@ -1721,7 +1701,7 @@
         <v>5874</v>
       </c>
       <c r="F35">
-        <v>0.58740000000000003</v>
+        <v>0.5874</v>
       </c>
       <c r="G35" t="s">
         <v>107</v>
@@ -1730,7 +1710,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
@@ -1747,7 +1727,7 @@
         <v>1526</v>
       </c>
       <c r="F36">
-        <v>0.15260000000000001</v>
+        <v>0.1526</v>
       </c>
       <c r="G36" t="s">
         <v>108</v>
@@ -1756,7 +1736,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
         <v>42</v>
       </c>
@@ -1773,7 +1753,7 @@
         <v>1526</v>
       </c>
       <c r="F37">
-        <v>0.15260000000000001</v>
+        <v>0.1526</v>
       </c>
       <c r="G37" t="s">
         <v>109</v>
@@ -1782,7 +1762,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
@@ -1799,7 +1779,7 @@
         <v>987</v>
       </c>
       <c r="F38">
-        <v>9.8699999999999996E-2</v>
+        <v>0.0987</v>
       </c>
       <c r="G38" t="s">
         <v>110</v>
@@ -1808,7 +1788,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
@@ -1834,7 +1814,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
@@ -1851,7 +1831,7 @@
         <v>8522</v>
       </c>
       <c r="F40">
-        <v>0.85219999999999996</v>
+        <v>0.8522</v>
       </c>
       <c r="G40" t="s">
         <v>112</v>
@@ -1860,7 +1840,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
         <v>46</v>
       </c>
@@ -1877,7 +1857,7 @@
         <v>8524</v>
       </c>
       <c r="F41">
-        <v>0.85240000000000005</v>
+        <v>0.8524</v>
       </c>
       <c r="G41" t="s">
         <v>113</v>
@@ -1886,7 +1866,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
@@ -1903,13 +1883,13 @@
         <v>142</v>
       </c>
       <c r="F42">
-        <v>1.4200000000000001E-2</v>
+        <v>0.0142</v>
       </c>
       <c r="H42" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
@@ -1926,7 +1906,7 @@
         <v>9371</v>
       </c>
       <c r="F43">
-        <v>0.93710000000000004</v>
+        <v>0.9371</v>
       </c>
       <c r="G43" t="s">
         <v>114</v>
@@ -1935,7 +1915,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
@@ -1952,13 +1932,13 @@
         <v>2461</v>
       </c>
       <c r="F44">
-        <v>0.24610000000000001</v>
+        <v>0.2461</v>
       </c>
       <c r="H44" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
@@ -1975,7 +1955,7 @@
         <v>2468</v>
       </c>
       <c r="F45">
-        <v>0.24679999999999999</v>
+        <v>0.2468</v>
       </c>
       <c r="G45" t="s">
         <v>115</v>
@@ -1984,7 +1964,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
@@ -2001,7 +1981,7 @@
         <v>2466</v>
       </c>
       <c r="F46">
-        <v>0.24660000000000001</v>
+        <v>0.2466</v>
       </c>
       <c r="G46" t="s">
         <v>115</v>
@@ -2010,7 +1990,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
         <v>52</v>
       </c>
@@ -2024,16 +2004,16 @@
         <v>89</v>
       </c>
       <c r="E47">
-        <v>3333</v>
+        <v>8436</v>
       </c>
       <c r="F47">
-        <v>0.33329999999999999</v>
+        <v>0.8436</v>
       </c>
       <c r="H47" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
@@ -2047,16 +2027,16 @@
         <v>89</v>
       </c>
       <c r="E48">
-        <v>3327</v>
+        <v>8573</v>
       </c>
       <c r="F48">
-        <v>0.3327</v>
+        <v>0.8573</v>
       </c>
       <c r="H48" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
@@ -2073,7 +2053,7 @@
         <v>7396</v>
       </c>
       <c r="F49">
-        <v>0.73960000000000004</v>
+        <v>0.7396</v>
       </c>
       <c r="G49" t="s">
         <v>116</v>
@@ -2082,7 +2062,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
@@ -2099,7 +2079,7 @@
         <v>7583</v>
       </c>
       <c r="F50">
-        <v>0.75829999999999997</v>
+        <v>0.7583</v>
       </c>
       <c r="G50" t="s">
         <v>117</v>
@@ -2108,7 +2088,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
@@ -2134,7 +2114,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
@@ -2151,7 +2131,7 @@
         <v>2245</v>
       </c>
       <c r="F52">
-        <v>0.22450000000000001</v>
+        <v>0.2245</v>
       </c>
       <c r="G52" t="s">
         <v>119</v>
@@ -2160,7 +2140,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
@@ -2183,7 +2163,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
         <v>59</v>
       </c>
@@ -2200,13 +2180,13 @@
         <v>1674</v>
       </c>
       <c r="F54">
-        <v>0.16739999999999999</v>
+        <v>0.1674</v>
       </c>
       <c r="H54" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
         <v>60</v>
       </c>
@@ -2223,7 +2203,7 @@
         <v>5337</v>
       </c>
       <c r="F55">
-        <v>0.53369999999999995</v>
+        <v>0.5337</v>
       </c>
       <c r="G55" t="s">
         <v>120</v>
@@ -2232,7 +2212,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
         <v>61</v>
       </c>
@@ -2255,7 +2235,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
         <v>62</v>
       </c>
@@ -2272,13 +2252,13 @@
         <v>5137</v>
       </c>
       <c r="F57">
-        <v>0.51370000000000005</v>
+        <v>0.5137</v>
       </c>
       <c r="H57" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
         <v>63</v>
       </c>
@@ -2295,7 +2275,7 @@
         <v>9347</v>
       </c>
       <c r="F58">
-        <v>0.93469999999999998</v>
+        <v>0.9347</v>
       </c>
       <c r="G58" t="s">
         <v>121</v>
@@ -2304,7 +2284,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
         <v>64</v>
       </c>
@@ -2321,7 +2301,7 @@
         <v>9347</v>
       </c>
       <c r="F59">
-        <v>0.93469999999999998</v>
+        <v>0.9347</v>
       </c>
       <c r="G59" t="s">
         <v>121</v>
@@ -2330,7 +2310,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -2347,13 +2327,13 @@
         <v>3420</v>
       </c>
       <c r="F60">
-        <v>0.34200000000000003</v>
+        <v>0.342</v>
       </c>
       <c r="H60" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
         <v>66</v>
       </c>
@@ -2370,7 +2350,7 @@
         <v>5086</v>
       </c>
       <c r="F61">
-        <v>0.50860000000000005</v>
+        <v>0.5086000000000001</v>
       </c>
       <c r="G61" t="s">
         <v>122</v>
@@ -2379,7 +2359,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
         <v>67</v>
       </c>
@@ -2405,7 +2385,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
         <v>68</v>
       </c>
@@ -2422,13 +2402,13 @@
         <v>6789</v>
       </c>
       <c r="F63">
-        <v>0.67889999999999995</v>
+        <v>0.6788999999999999</v>
       </c>
       <c r="H63" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8">
       <c r="A64" s="1" t="s">
         <v>69</v>
       </c>
@@ -2445,13 +2425,13 @@
         <v>2765</v>
       </c>
       <c r="F64">
-        <v>0.27650000000000002</v>
+        <v>0.2765</v>
       </c>
       <c r="H64" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8">
       <c r="A65" s="1" t="s">
         <v>70</v>
       </c>
@@ -2468,13 +2448,13 @@
         <v>2765</v>
       </c>
       <c r="F65">
-        <v>0.27650000000000002</v>
+        <v>0.2765</v>
       </c>
       <c r="H65" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8">
       <c r="A66" s="1" t="s">
         <v>71</v>
       </c>
@@ -2491,7 +2471,7 @@
         <v>6920</v>
       </c>
       <c r="F66">
-        <v>0.69199999999999995</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="G66" t="s">
         <v>124</v>
@@ -2500,7 +2480,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8">
       <c r="A67" s="1" t="s">
         <v>72</v>
       </c>
@@ -2517,13 +2497,13 @@
         <v>5059</v>
       </c>
       <c r="F67">
-        <v>0.50590000000000002</v>
+        <v>0.5059</v>
       </c>
       <c r="H67" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8">
       <c r="A68" s="1" t="s">
         <v>73</v>
       </c>
@@ -2540,7 +2520,7 @@
         <v>7109</v>
       </c>
       <c r="F68">
-        <v>0.71089999999999998</v>
+        <v>0.7109</v>
       </c>
       <c r="G68" t="s">
         <v>125</v>
@@ -2549,7 +2529,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8">
       <c r="A69" s="1" t="s">
         <v>74</v>
       </c>
@@ -2566,13 +2546,13 @@
         <v>5059</v>
       </c>
       <c r="F69">
-        <v>0.50590000000000002</v>
+        <v>0.5059</v>
       </c>
       <c r="H69" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8">
       <c r="A70" s="1" t="s">
         <v>75</v>
       </c>
@@ -2589,7 +2569,7 @@
         <v>8634</v>
       </c>
       <c r="F70">
-        <v>0.86339999999999995</v>
+        <v>0.8633999999999999</v>
       </c>
       <c r="G70" t="s">
         <v>126</v>
@@ -2598,7 +2578,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8">
       <c r="A71" s="1" t="s">
         <v>76</v>
       </c>
@@ -2615,13 +2595,13 @@
         <v>4235</v>
       </c>
       <c r="F71">
-        <v>0.42349999999999999</v>
+        <v>0.4235</v>
       </c>
       <c r="H71" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8">
       <c r="A72" s="1" t="s">
         <v>77</v>
       </c>
@@ -2638,13 +2618,13 @@
         <v>4233</v>
       </c>
       <c r="F72">
-        <v>0.42330000000000001</v>
+        <v>0.4233</v>
       </c>
       <c r="H72" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8">
       <c r="A73" s="1" t="s">
         <v>78</v>
       </c>
@@ -2661,7 +2641,7 @@
         <v>4460</v>
       </c>
       <c r="F73">
-        <v>0.44600000000000001</v>
+        <v>0.446</v>
       </c>
       <c r="G73" t="s">
         <v>127</v>
@@ -2670,7 +2650,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8">
       <c r="A74" s="1" t="s">
         <v>79</v>
       </c>
@@ -2687,7 +2667,7 @@
         <v>4275</v>
       </c>
       <c r="F74">
-        <v>0.42749999999999999</v>
+        <v>0.4275</v>
       </c>
       <c r="G74" t="s">
         <v>128</v>
@@ -2696,7 +2676,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8">
       <c r="A75" s="1" t="s">
         <v>80</v>
       </c>
@@ -2713,7 +2693,7 @@
         <v>5072</v>
       </c>
       <c r="F75">
-        <v>0.50719999999999998</v>
+        <v>0.5072</v>
       </c>
       <c r="G75" t="s">
         <v>129</v>
@@ -2722,7 +2702,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8">
       <c r="A76" s="1" t="s">
         <v>81</v>
       </c>
@@ -2739,13 +2719,13 @@
         <v>4232</v>
       </c>
       <c r="F76">
-        <v>0.42320000000000002</v>
+        <v>0.4232</v>
       </c>
       <c r="H76" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8">
       <c r="A77" s="1" t="s">
         <v>82</v>
       </c>
@@ -2762,13 +2742,13 @@
         <v>5158</v>
       </c>
       <c r="F77">
-        <v>0.51580000000000004</v>
+        <v>0.5158</v>
       </c>
       <c r="H77" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8">
       <c r="A78" s="1" t="s">
         <v>83</v>
       </c>
@@ -2785,7 +2765,7 @@
         <v>8304</v>
       </c>
       <c r="F78">
-        <v>0.83040000000000003</v>
+        <v>0.8304</v>
       </c>
       <c r="H78" t="s">
         <v>153</v>

</xml_diff>